<commit_message>
docs done for now
</commit_message>
<xml_diff>
--- a/GanttChart.xlsx
+++ b/GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\FinalYearProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E4F385-6EAA-4F88-AF3D-210894BE464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE85EAEE-5284-4510-ABAB-20425D844D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{660A0054-D622-4A55-8AA9-855CE31CB824}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>OCTOBER</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>DEADLINE</t>
+  </si>
+  <si>
+    <t>FEBRUARY</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>MARCH</t>
+  </si>
+  <si>
+    <t>DEMO</t>
   </si>
 </sst>
 </file>
@@ -101,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +156,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -247,30 +271,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -283,15 +283,6 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -307,11 +298,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -329,14 +357,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -652,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F7DC8F-9FF1-48D0-A090-2CD04B34C423}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +698,7 @@
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -693,8 +728,20 @@
       </c>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -754,8 +801,32 @@
       <c r="U2" s="10">
         <v>44955</v>
       </c>
+      <c r="V2" s="25">
+        <v>44962</v>
+      </c>
+      <c r="W2" s="25">
+        <v>44969</v>
+      </c>
+      <c r="X2" s="25">
+        <v>44976</v>
+      </c>
+      <c r="Y2" s="25">
+        <v>44983</v>
+      </c>
+      <c r="Z2" s="28">
+        <v>44989</v>
+      </c>
+      <c r="AA2" s="28">
+        <v>44996</v>
+      </c>
+      <c r="AB2" s="28">
+        <v>45003</v>
+      </c>
+      <c r="AC2" s="28">
+        <v>45010</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -763,11 +834,14 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="14"/>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="29" t="s">
         <v>12</v>
       </c>
+      <c r="R3" s="29" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -777,12 +851,13 @@
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="3" t="s">
+      <c r="M4" s="15"/>
+      <c r="N4" s="30" t="s">
         <v>13</v>
       </c>
+      <c r="R4" s="30"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -792,19 +867,21 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="3"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="30"/>
+      <c r="R5" s="30"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-      <c r="N6" s="3"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
+      <c r="N6" s="30"/>
+      <c r="R6" s="30"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -815,47 +892,73 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="U7" s="21"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="14"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="14"/>
+      <c r="U7" s="26"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="11"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="R8" s="19"/>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
-      <c r="U8" s="13"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="13"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="20"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="18"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>